<commit_message>
menambah video ke dalam slide
</commit_message>
<xml_diff>
--- a/src/BurnDownChart.xlsx
+++ b/src/BurnDownChart.xlsx
@@ -681,7 +681,7 @@
                   <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -725,11 +725,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2108821632"/>
-        <c:axId val="-2108820544"/>
+        <c:axId val="-1917763024"/>
+        <c:axId val="-1917753232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2108821632"/>
+        <c:axId val="-1917763024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +739,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108820544"/>
+        <c:crossAx val="-1917753232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -747,7 +747,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108820544"/>
+        <c:axId val="-1917753232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,7 +757,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="-2108821632"/>
+        <c:crossAx val="-1917763024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="D24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50366,7 +50366,9 @@
       <c r="G6" s="4">
         <v>0</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -50397,7 +50399,9 @@
       <c r="G7" s="4">
         <v>0</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="1"/>
@@ -50428,7 +50432,9 @@
       <c r="G8" s="4">
         <v>0</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="8"/>
@@ -50459,7 +50465,9 @@
       <c r="G9" s="4">
         <v>0</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="8"/>
@@ -50490,7 +50498,9 @@
       <c r="G10" s="4">
         <v>5</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="8"/>
@@ -50521,7 +50531,9 @@
       <c r="G11" s="4">
         <v>6</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4">
+        <v>6</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="8"/>
@@ -50552,7 +50564,9 @@
       <c r="G12" s="4">
         <v>6</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4">
+        <v>6</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -50583,7 +50597,9 @@
       <c r="G13" s="4">
         <v>6</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4">
+        <v>6</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -50614,7 +50630,9 @@
       <c r="G14" s="4">
         <v>6</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4">
+        <v>6</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="1"/>
@@ -50645,7 +50663,9 @@
       <c r="G15" s="4">
         <v>6</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4">
+        <v>6</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="8"/>
@@ -50676,7 +50696,9 @@
       <c r="G16" s="4">
         <v>6</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4">
+        <v>6</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="8"/>
@@ -50707,7 +50729,9 @@
       <c r="G17" s="4">
         <v>6</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4">
+        <v>6</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -50738,7 +50762,9 @@
       <c r="G18" s="8">
         <v>6</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="4">
+        <v>6</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="21"/>
       <c r="K18" s="4"/>
@@ -50769,7 +50795,9 @@
       <c r="G19" s="8">
         <v>6</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="4">
+        <v>6</v>
+      </c>
       <c r="I19" s="8"/>
       <c r="J19" s="9"/>
       <c r="K19" s="8"/>
@@ -50800,7 +50828,9 @@
       <c r="G20" s="4">
         <v>6</v>
       </c>
-      <c r="H20" s="21"/>
+      <c r="H20" s="4">
+        <v>6</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="21"/>
       <c r="K20" s="4"/>
@@ -50831,7 +50861,9 @@
       <c r="G21" s="18">
         <v>6</v>
       </c>
-      <c r="H21" s="12"/>
+      <c r="H21" s="4">
+        <v>6</v>
+      </c>
       <c r="I21" s="18"/>
       <c r="J21" s="12"/>
       <c r="K21" s="18"/>
@@ -50862,7 +50894,9 @@
       <c r="G22" s="4">
         <v>6</v>
       </c>
-      <c r="H22" s="21"/>
+      <c r="H22" s="4">
+        <v>6</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="21"/>
       <c r="K22" s="4"/>
@@ -50893,7 +50927,9 @@
       <c r="G23" s="18">
         <v>6</v>
       </c>
-      <c r="H23" s="12"/>
+      <c r="H23" s="4">
+        <v>6</v>
+      </c>
       <c r="I23" s="18"/>
       <c r="J23" s="12"/>
       <c r="K23" s="18"/>
@@ -50924,7 +50960,9 @@
       <c r="G24" s="4">
         <v>6</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="4">
+        <v>6</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="21"/>
       <c r="K24" s="4"/>
@@ -50955,7 +50993,9 @@
       <c r="G25" s="4">
         <v>2</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4">
+        <v>2</v>
+      </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -51050,7 +51090,7 @@
       </c>
       <c r="H27" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="I27" s="4">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
create "Matte Painting" slide
</commit_message>
<xml_diff>
--- a/src/BurnDownChart.xlsx
+++ b/src/BurnDownChart.xlsx
@@ -1,22 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Presentasi TKPPL\src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -26,7 +19,7 @@
     <author>mkg</author>
   </authors>
   <commentList>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -289,63 +282,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -373,32 +315,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -413,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -441,9 +357,6 @@
     <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -453,28 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
@@ -483,13 +375,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -523,7 +415,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-AU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -684,31 +576,31 @@
                   <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,11 +617,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1917763024"/>
-        <c:axId val="-1917753232"/>
+        <c:axId val="73872896"/>
+        <c:axId val="73874432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1917763024"/>
+        <c:axId val="73872896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +631,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1917753232"/>
+        <c:crossAx val="73874432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -747,7 +639,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1917753232"/>
+        <c:axId val="73874432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,7 +649,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="-1917763024"/>
+        <c:crossAx val="73872896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1101,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,12 +1009,12 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -33890,14 +33782,14 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -50369,15 +50261,42 @@
       <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:Q6" si="0">IF(H6=0,0,H6)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
@@ -50402,15 +50321,42 @@
       <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="I7" s="4">
+        <f t="shared" ref="I7:Q7" si="1">IF(H7=0,0,H7)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
@@ -50435,15 +50381,42 @@
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
+      <c r="I8" s="4">
+        <f t="shared" ref="I8:Q8" si="2">IF(H8=0,0,H8)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
@@ -50468,15 +50441,42 @@
       <c r="H9" s="4">
         <v>0</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="I9" s="4">
+        <f t="shared" ref="I9:Q9" si="3">IF(H9=0,0,H9)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <f>IF(I9=0,0,I9)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" ref="K9:Q9" si="4">IF(J9=0,0,J9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
@@ -50501,15 +50501,41 @@
       <c r="H10" s="4">
         <v>1</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" ref="I10:Q10" si="5">IF(I10=0,0,I10)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
@@ -50534,15 +50560,41 @@
       <c r="H11" s="4">
         <v>6</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
+      <c r="I11" s="4">
+        <v>3</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" ref="I11:Q11" si="6">IF(I11=0,0,I11)</f>
+        <v>3</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
@@ -50567,15 +50619,41 @@
       <c r="H12" s="4">
         <v>6</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
+      <c r="I12" s="4">
+        <v>3</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" ref="I12:Q12" si="7">IF(I12=0,0,I12)</f>
+        <v>3</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
@@ -50600,15 +50678,41 @@
       <c r="H13" s="4">
         <v>6</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
+      <c r="I13" s="4">
+        <v>3</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" ref="I13:Q13" si="8">IF(I13=0,0,I13)</f>
+        <v>3</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
@@ -50633,15 +50737,41 @@
       <c r="H14" s="4">
         <v>6</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
+      <c r="I14" s="4">
+        <v>3</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" ref="I14:Q14" si="9">IF(I14=0,0,I14)</f>
+        <v>3</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
@@ -50666,15 +50796,42 @@
       <c r="H15" s="4">
         <v>6</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
+      <c r="I15" s="4">
+        <f t="shared" ref="I15:Q15" si="10">IF(H15=0,0,H15)</f>
+        <v>6</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
@@ -50699,15 +50856,42 @@
       <c r="H16" s="4">
         <v>6</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
+      <c r="I16" s="4">
+        <f t="shared" ref="I16:Q16" si="11">IF(H16=0,0,H16)</f>
+        <v>6</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="M16" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="N16" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="O16" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="P16" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="Q16" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
@@ -50732,15 +50916,42 @@
       <c r="H17" s="4">
         <v>6</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
+      <c r="I17" s="4">
+        <f t="shared" ref="I17:Q17" si="12">IF(H17=0,0,H17)</f>
+        <v>6</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="O17" s="4">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
@@ -50752,7 +50963,7 @@
       <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="8">
         <v>6</v>
       </c>
@@ -50765,15 +50976,42 @@
       <c r="H18" s="4">
         <v>6</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="11"/>
+      <c r="I18" s="4">
+        <f t="shared" ref="I18:Q18" si="13">IF(H18=0,0,H18)</f>
+        <v>6</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="M18" s="4">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="N18" s="4">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="O18" s="4">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="P18" s="4">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="Q18" s="4">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
@@ -50782,10 +51020,10 @@
       <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="23"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="8">
         <v>6</v>
       </c>
@@ -50798,15 +51036,42 @@
       <c r="H19" s="4">
         <v>6</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="11"/>
+      <c r="I19" s="4">
+        <f t="shared" ref="I19:Q19" si="14">IF(H19=0,0,H19)</f>
+        <v>6</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="O19" s="4">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="P19" s="4">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
@@ -50815,14 +51080,14 @@
       <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="4">
         <v>6</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="13">
         <v>6</v>
       </c>
       <c r="G20" s="4">
@@ -50831,15 +51096,42 @@
       <c r="H20" s="4">
         <v>6</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="20"/>
+      <c r="I20" s="4">
+        <f t="shared" ref="I20:Q20" si="15">IF(H20=0,0,H20)</f>
+        <v>6</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="M20" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="N20" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="O20" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="P20" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="Q20" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
@@ -50848,31 +51140,58 @@
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="18">
+      <c r="D21" s="19"/>
+      <c r="E21" s="12">
         <v>6</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="11">
         <v>6</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="12">
         <v>6</v>
       </c>
       <c r="H21" s="4">
         <v>6</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="13"/>
+      <c r="I21" s="4">
+        <f t="shared" ref="I21:Q21" si="16">IF(H21=0,0,H21)</f>
+        <v>6</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
@@ -50881,14 +51200,14 @@
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="4">
         <v>6</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="13">
         <v>6</v>
       </c>
       <c r="G22" s="4">
@@ -50897,15 +51216,42 @@
       <c r="H22" s="4">
         <v>6</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="20"/>
+      <c r="I22" s="4">
+        <f t="shared" ref="I22:Q22" si="17">IF(H22=0,0,H22)</f>
+        <v>6</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="M22" s="4">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="O22" s="4">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
@@ -50914,31 +51260,58 @@
       <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="18">
+      <c r="D23" s="19"/>
+      <c r="E23" s="12">
         <v>6</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="11">
         <v>6</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="12">
         <v>6</v>
       </c>
       <c r="H23" s="4">
         <v>6</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="16"/>
+      <c r="I23" s="4">
+        <f t="shared" ref="I23:Q23" si="18">IF(H23=0,0,H23)</f>
+        <v>6</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="M23" s="4">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="O23" s="4">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="P23" s="4">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
@@ -50947,14 +51320,14 @@
       <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="4">
         <v>6</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="13">
         <v>6</v>
       </c>
       <c r="G24" s="4">
@@ -50963,15 +51336,42 @@
       <c r="H24" s="4">
         <v>6</v>
       </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="16"/>
+      <c r="I24" s="4">
+        <f t="shared" ref="I24:Q24" si="19">IF(H24=0,0,H24)</f>
+        <v>6</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="L24" s="4">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="M24" s="4">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="N24" s="4">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="O24" s="4">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="P24" s="4">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="Q24" s="4">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
@@ -50996,25 +51396,52 @@
       <c r="H25" s="4">
         <v>2</v>
       </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
+      <c r="I25" s="4">
+        <f t="shared" ref="I25:Q25" si="20">IF(H25=0,0,H25)</f>
+        <v>2</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="M25" s="4">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="O25" s="4">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="P25" s="4">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="Q25" s="4">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="4">
         <f>SUM(E6:E25)</f>
         <v>104</v>
@@ -51024,43 +51451,43 @@
         <v>95</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" ref="G26:P26" si="0">ROUND(F26-$E$26/12,0)</f>
+        <f t="shared" ref="G26:P26" si="21">ROUND(F26-$E$26/12,0)</f>
         <v>86</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>77</v>
       </c>
       <c r="I26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>68</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="K26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>50</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>41</v>
       </c>
       <c r="M26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>32</v>
       </c>
       <c r="N26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>23</v>
       </c>
       <c r="O26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>14</v>
       </c>
       <c r="P26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="21"/>
         <v>5</v>
       </c>
       <c r="Q26" s="8">
@@ -51071,62 +51498,62 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="4">
         <f>SUM(E6:E25)</f>
         <v>104</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" ref="F27:Q27" si="1">SUM(F6:F25)</f>
+        <f t="shared" ref="F27:Q27" si="22">SUM(F6:F25)</f>
         <v>97</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="22"/>
         <v>91</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="22"/>
         <v>87</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="L27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="M27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="O27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="P27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="Q27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>74</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -51756,28 +52183,4 @@
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>